<commit_message>
- Added keyword options to multipole mixing rule - Added check that polarizability is bounded - Added global optimization method for single calculation of given parameters - Added factory method for objective function to data_classes, default: squared-average-deviation - thermodynamics.calc_types update to allow one composition to be used for a series of temperature values
</commit_message>
<xml_diff>
--- a/despasito/examples/hexane_heptane/Comparison.xlsx
+++ b/despasito/examples/hexane_heptane/Comparison.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Jennifer/bin/DESPASITO/despasito/despasito/examples/hexane_heptane/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9DA0C31-1A63-1044-A51C-4E2D2BC1A5B2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECE3B98B-0221-C54F-AF22-0881608596F0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3180" yWindow="460" windowWidth="22180" windowHeight="10980" xr2:uid="{A45715C8-7133-A340-ADEA-03B6CBD95D09}"/>
+    <workbookView xWindow="10280" yWindow="460" windowWidth="24240" windowHeight="14420" xr2:uid="{A45715C8-7133-A340-ADEA-03B6CBD95D09}"/>
   </bookViews>
   <sheets>
     <sheet name="New Derivative" sheetId="2" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="22">
   <si>
     <t># P [Pa]</t>
   </si>
@@ -94,13 +94,16 @@
   </si>
   <si>
     <t>JIT</t>
+  </si>
+  <si>
+    <t>Muller quadrature</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -109,12 +112,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -129,8 +138,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -445,13 +456,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71E2719B-E892-E04B-BE13-036557DDA31C}">
-  <dimension ref="A1:R18"/>
+  <dimension ref="A1:R24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="K29" sqref="K29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="22" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="2.5" bestFit="1" customWidth="1"/>
@@ -461,7 +472,7 @@
     <col min="11" max="11" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18">
       <c r="C1" t="s">
         <v>0</v>
       </c>
@@ -505,7 +516,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:18">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -533,19 +544,19 @@
       <c r="I2">
         <v>0.20355023555104301</v>
       </c>
-      <c r="J2">
+      <c r="J2" s="1">
         <f>1/G2</f>
         <v>1.4405468088380129E-4</v>
       </c>
-      <c r="K2">
+      <c r="K2" s="1">
         <f t="shared" ref="K2:L5" si="0">LN(H2)</f>
         <v>-0.51969368207839428</v>
       </c>
-      <c r="L2">
+      <c r="L2" s="1">
         <f t="shared" si="0"/>
         <v>-1.5918424468191639</v>
       </c>
-      <c r="M2">
+      <c r="M2" s="2">
         <v>1.44356E-4</v>
       </c>
       <c r="N2">
@@ -567,7 +578,7 @@
         <v>-1.5984146121552851</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:18">
       <c r="B3" t="s">
         <v>8</v>
       </c>
@@ -592,19 +603,19 @@
       <c r="I3">
         <v>0.94823020047261597</v>
       </c>
-      <c r="J3">
+      <c r="J3" s="1">
         <f>1/G3</f>
         <v>2.5303033430040148E-2</v>
       </c>
-      <c r="K3">
+      <c r="K3" s="1">
         <f t="shared" si="0"/>
         <v>-3.8411982151552206E-2</v>
       </c>
-      <c r="L3">
+      <c r="L3" s="1">
         <f t="shared" si="0"/>
         <v>-5.3157978702181911E-2</v>
       </c>
-      <c r="M3">
+      <c r="M3" s="2">
         <v>2.5304E-2</v>
       </c>
       <c r="N3">
@@ -626,7 +637,7 @@
         <v>0.16577859842078818</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -688,7 +699,7 @@
         <v>10.214072634352384</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:18">
       <c r="B5" t="s">
         <v>8</v>
       </c>
@@ -747,12 +758,12 @@
         <v>2.3627822397961649</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:18">
       <c r="A6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:18">
       <c r="C7" t="s">
         <v>0</v>
       </c>
@@ -796,7 +807,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:18">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -858,7 +869,7 @@
         <v>1.8071282816070466</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:18">
       <c r="B9" t="s">
         <v>8</v>
       </c>
@@ -917,7 +928,7 @@
         <v>0.12082250098293403</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:18">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -979,7 +990,7 @@
         <v>13.351183559446969</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:18">
       <c r="B11" t="s">
         <v>8</v>
       </c>
@@ -1038,12 +1049,12 @@
         <v>2.3170652533766951</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:18">
       <c r="A13" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:18">
       <c r="C14" t="s">
         <v>0</v>
       </c>
@@ -1087,7 +1098,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:18">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -1120,11 +1131,11 @@
         <v>1.5293177573054521E-4</v>
       </c>
       <c r="K15">
-        <f t="shared" ref="K15:K18" si="6">LN(H15)</f>
+        <f>LN(H15)</f>
         <v>-1.4281231162478876</v>
       </c>
       <c r="L15">
-        <f t="shared" ref="L15:L18" si="7">LN(I15)</f>
+        <f t="shared" ref="L15:L18" si="6">LN(I15)</f>
         <v>-2.4703933324780065</v>
       </c>
       <c r="M15">
@@ -1149,7 +1160,7 @@
         <v>52.710226400321858</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:18">
       <c r="B16" t="s">
         <v>8</v>
       </c>
@@ -1179,11 +1190,11 @@
         <v>2.4152040587823918E-2</v>
       </c>
       <c r="K16">
+        <f t="shared" ref="K15:K18" si="7">LN(H16)</f>
+        <v>-3.1737465565117424</v>
+      </c>
+      <c r="L16">
         <f t="shared" si="6"/>
-        <v>-3.1737465565117424</v>
-      </c>
-      <c r="L16">
-        <f t="shared" si="7"/>
         <v>-3.4482982358288941</v>
       </c>
       <c r="M16">
@@ -1208,7 +1219,7 @@
         <v>6397.6412960785647</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:18">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -1241,11 +1252,11 @@
         <v>1.5544070051078834E-4</v>
       </c>
       <c r="K17">
+        <f t="shared" si="7"/>
+        <v>-1.7193046016118052</v>
+      </c>
+      <c r="L17">
         <f t="shared" si="6"/>
-        <v>-1.7193046016118052</v>
-      </c>
-      <c r="L17">
-        <f t="shared" si="7"/>
         <v>-2.974419367708435</v>
       </c>
       <c r="M17">
@@ -1270,7 +1281,7 @@
         <v>83.867179805182374</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:18">
       <c r="B18" t="s">
         <v>8</v>
       </c>
@@ -1300,11 +1311,11 @@
         <v>2.4195093026562954E-2</v>
       </c>
       <c r="K18">
+        <f t="shared" si="7"/>
+        <v>-3.2975381853750054</v>
+      </c>
+      <c r="L18">
         <f t="shared" si="6"/>
-        <v>-3.2975381853750054</v>
-      </c>
-      <c r="L18">
-        <f t="shared" si="7"/>
         <v>-4.1491662271434624</v>
       </c>
       <c r="M18">
@@ -1327,6 +1338,253 @@
       <c r="R18">
         <f t="shared" si="10"/>
         <v>7718.2894802024921</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18">
+      <c r="A19" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18">
+      <c r="A20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B20" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" t="s">
+        <v>9</v>
+      </c>
+      <c r="D20">
+        <v>320</v>
+      </c>
+      <c r="E20">
+        <v>0.4</v>
+      </c>
+      <c r="F20">
+        <v>0.6</v>
+      </c>
+      <c r="G20">
+        <v>6934.7742909341096</v>
+      </c>
+      <c r="H20">
+        <v>0.59975345894936405</v>
+      </c>
+      <c r="I20">
+        <v>0.198377670948923</v>
+      </c>
+      <c r="J20" s="1">
+        <f>1/G20</f>
+        <v>1.4420079991749822E-4</v>
+      </c>
+      <c r="K20" s="1">
+        <f>LN(H20)</f>
+        <v>-0.51123660996030784</v>
+      </c>
+      <c r="L20" s="1">
+        <f t="shared" ref="L20:L21" si="11">LN(I20)</f>
+        <v>-1.6175826360854459</v>
+      </c>
+      <c r="M20">
+        <v>1.44356E-4</v>
+      </c>
+      <c r="N20">
+        <v>-0.50790000000000002</v>
+      </c>
+      <c r="O20">
+        <v>-1.6176999999999999</v>
+      </c>
+      <c r="P20">
+        <f>(J20-M20)/M20*100</f>
+        <v>-0.1075120414127456</v>
+      </c>
+      <c r="Q20">
+        <f>(K20-N20)/N20*100</f>
+        <v>0.65694230366367856</v>
+      </c>
+      <c r="R20">
+        <f>(L20-O20)/O20*100</f>
+        <v>-7.2549863728731878E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18">
+      <c r="B21" t="s">
+        <v>8</v>
+      </c>
+      <c r="C21" t="s">
+        <v>9</v>
+      </c>
+      <c r="D21">
+        <v>320</v>
+      </c>
+      <c r="E21">
+        <v>0.4</v>
+      </c>
+      <c r="F21">
+        <v>0.6</v>
+      </c>
+      <c r="G21">
+        <v>39.518709018646398</v>
+      </c>
+      <c r="H21">
+        <v>0.96238064443974802</v>
+      </c>
+      <c r="I21">
+        <v>0.94829976904272095</v>
+      </c>
+      <c r="J21" s="1">
+        <f>1/G21</f>
+        <v>2.5304470333992003E-2</v>
+      </c>
+      <c r="K21" s="1">
+        <f t="shared" ref="K21" si="12">LN(H21)</f>
+        <v>-3.8345226286434976E-2</v>
+      </c>
+      <c r="L21" s="1">
+        <f t="shared" si="11"/>
+        <v>-5.3084614641234366E-2</v>
+      </c>
+      <c r="M21">
+        <v>2.5304E-2</v>
+      </c>
+      <c r="N21">
+        <v>-3.832E-2</v>
+      </c>
+      <c r="O21">
+        <v>-5.3069999999999999E-2</v>
+      </c>
+      <c r="P21">
+        <f t="shared" ref="P21" si="13">(J21-M21)/M21*100</f>
+        <v>1.8587337654249751E-3</v>
+      </c>
+      <c r="Q21">
+        <f t="shared" ref="Q21" si="14">(K21-N21)/N21*100</f>
+        <v>6.5830601343883494E-2</v>
+      </c>
+      <c r="R21">
+        <f t="shared" ref="R21" si="15">(L21-O21)/O21*100</f>
+        <v>2.7538423279380605E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18">
+      <c r="A23" t="s">
+        <v>13</v>
+      </c>
+      <c r="B23" t="s">
+        <v>7</v>
+      </c>
+      <c r="C23" t="s">
+        <v>9</v>
+      </c>
+      <c r="D23">
+        <v>320</v>
+      </c>
+      <c r="E23">
+        <v>0.4</v>
+      </c>
+      <c r="F23">
+        <v>0.6</v>
+      </c>
+      <c r="G23">
+        <v>6926.8573690000003</v>
+      </c>
+      <c r="H23">
+        <v>0.60173382348734095</v>
+      </c>
+      <c r="I23">
+        <v>0.198336089672183</v>
+      </c>
+      <c r="J23" s="1">
+        <f>1/G23</f>
+        <v>1.4436561152180409E-4</v>
+      </c>
+      <c r="K23" s="1">
+        <f>LN(H23)</f>
+        <v>-0.50794008512758904</v>
+      </c>
+      <c r="L23" s="1">
+        <f t="shared" ref="L23:L24" si="16">LN(I23)</f>
+        <v>-1.6177922646943814</v>
+      </c>
+      <c r="M23">
+        <v>1.44356E-4</v>
+      </c>
+      <c r="N23">
+        <v>-0.50790000000000002</v>
+      </c>
+      <c r="O23">
+        <v>-1.6176999999999999</v>
+      </c>
+      <c r="P23">
+        <f>(J23-M23)/M23*100</f>
+        <v>6.6582073513355442E-3</v>
+      </c>
+      <c r="Q23">
+        <f>(K23-N23)/N23*100</f>
+        <v>7.892326755073429E-3</v>
+      </c>
+      <c r="R23">
+        <f>(L23-O23)/O23*100</f>
+        <v>5.7034489943441503E-3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18">
+      <c r="B24" t="s">
+        <v>8</v>
+      </c>
+      <c r="C24" t="s">
+        <v>9</v>
+      </c>
+      <c r="D24">
+        <v>320</v>
+      </c>
+      <c r="E24">
+        <v>0.4</v>
+      </c>
+      <c r="F24">
+        <v>0.6</v>
+      </c>
+      <c r="G24">
+        <v>39.518145643857302</v>
+      </c>
+      <c r="H24">
+        <v>0.96239830678025595</v>
+      </c>
+      <c r="I24">
+        <v>0.94831340746703496</v>
+      </c>
+      <c r="J24" s="1">
+        <f>1/G24</f>
+        <v>2.5304831077149492E-2</v>
+      </c>
+      <c r="K24" s="1">
+        <f t="shared" ref="K24" si="17">LN(H24)</f>
+        <v>-3.8326873695352003E-2</v>
+      </c>
+      <c r="L24" s="1">
+        <f t="shared" si="16"/>
+        <v>-5.3070232768870344E-2</v>
+      </c>
+      <c r="M24">
+        <v>2.5304E-2</v>
+      </c>
+      <c r="N24">
+        <v>-3.832E-2</v>
+      </c>
+      <c r="O24">
+        <v>-5.3069999999999999E-2</v>
+      </c>
+      <c r="P24">
+        <f t="shared" ref="P24" si="18">(J24-M24)/M24*100</f>
+        <v>3.2843706508512683E-3</v>
+      </c>
+      <c r="Q24">
+        <f t="shared" ref="Q24" si="19">(K24-N24)/N24*100</f>
+        <v>1.7937618350737636E-2</v>
+      </c>
+      <c r="R24">
+        <f t="shared" ref="R24" si="20">(L24-O24)/O24*100</f>
+        <v>4.386072552198589E-4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>